<commit_message>
update for A1-A20 tasks
</commit_message>
<xml_diff>
--- a/NovelKalinin/evidence.xlsx
+++ b/NovelKalinin/evidence.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>TxHash</t>
   </si>
@@ -57,27 +57,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -172,6 +157,159 @@
   </si>
   <si>
     <t>7B6B496F98DB75F86BD168E19A6F2BB9541FA2FB6BAB8FEC00EF8A807FA4E676</t>
+  </si>
+  <si>
+    <t>ibc/6B9B16E53838B399456E27FA4DD203F3C61A84A74E08C39B36317358952EC0FA</t>
+  </si>
+  <si>
+    <t>infinity007</t>
+  </si>
+  <si>
+    <t>ibc/E46AF80253FBBC0E305135601D8B351A8BED393935DFAE0AB5A2D0C020BFD8B0</t>
+  </si>
+  <si>
+    <t>infinity008</t>
+  </si>
+  <si>
+    <t>ibc/CB031F7A67D02E6A80927310CE962DA24430E48162F7FC968097BE0E3F870AF5</t>
+  </si>
+  <si>
+    <t>infinity009</t>
+  </si>
+  <si>
+    <t>ibc/0DF228C531E522806241E96E5407BCBC3FDF890FC4A28D2436B5DA5423FB3C5D</t>
+  </si>
+  <si>
+    <t>infinity0010</t>
+  </si>
+  <si>
+    <t>ibc/BCBD4B5E86544F1104539E2DFE5DD5547E7257637222217111772451F629D3BC</t>
+  </si>
+  <si>
+    <t>infinity0011</t>
+  </si>
+  <si>
+    <t>ibc/43EF1C58A5288F1C7E1B9C9CBEB07CCB06151E10FFCF74DBEDF1E8AC8AAC45A5</t>
+  </si>
+  <si>
+    <t>infinity0012</t>
+  </si>
+  <si>
+    <t>CCF2DDC43DCD246005B89E2E1185F193B807C284EDD913F8C59AF3A619859FA7</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>E3B95DB374E2F2C9B14F1A9061E06ADDCB0B0246A7E73F4443E5E0FAA644295A</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>C3DCF067202DCF09B87244CD417077950FE1560C10052867781B244A4EACA3D0</t>
+  </si>
+  <si>
+    <t>2F6DEB1D1FE38D4733149B9BC96535BE33BEAF2F49CCF3C2B75CB1A361A3F484</t>
+  </si>
+  <si>
+    <t>FD90A8C4AD7BD81EC3EE5F155E5720FAE785BFE70621E92CE0057F5DE36918DD</t>
+  </si>
+  <si>
+    <t>6849FEAA46577FBA244248787F751840D774908B39F9B18C71D7CFD4B8EE7200</t>
+  </si>
+  <si>
+    <t>9FC6342AC59520E39C6C56B709908FD282A5FCEC2300590CCB35A264CB6EAF57</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>85731B40A3B6253FF88830FE2D4BA25886BD108FC297F3148A889EFD484F610A</t>
+  </si>
+  <si>
+    <t>56E91B56C948BA49E7C4E84470F176E866A0E687FC2C3150B035A56447C4F22E</t>
+  </si>
+  <si>
+    <t>62B90DB4FA2977868897A2AB1C0BD2B039B87E118C6FE1886546053964B886A1</t>
+  </si>
+  <si>
+    <t>7FF0C77347A7EFCFE111CA1E5244CD5926A2ADC15E5DA0857973972D60131B73</t>
+  </si>
+  <si>
+    <t>1ABA7FBA702952FAAB416BD4F8232BAE0D91CD4C926F2BB1E5F80F8EBA1AF08F</t>
+  </si>
+  <si>
+    <t>7A90FE81E80B027441456206558B63065E3916FF0FB2A28D3BCB8545F2C431EC</t>
+  </si>
+  <si>
+    <t>1024EDCF587648853578B8BB9B1009901AF3360E355893BF4D1C7DE5ABCC9C8D</t>
+  </si>
+  <si>
+    <t>7B8A8830F57980F1C26B897A89906F8CA621430DC4AC45CE582970867444AE2D</t>
+  </si>
+  <si>
+    <t>4AAE97B1044B6396EB44680FDF8216B6A7C3A692D8746C97434C444F5D4DCE0F</t>
+  </si>
+  <si>
+    <t>EA7A7EDBE55E275D944FE2AA6D230D44175D0264D765FE2231B446DC714A68CD</t>
+  </si>
+  <si>
+    <t>D4A91DFB32B9AF0F7E8221514AAB5B8B76DC1B23E9E0B19B9EBBB980F32409AB</t>
+  </si>
+  <si>
+    <t>9F75D464AE0134A4657886E874B582CB7A7C21CCC96D6466CE134539375AFE3F</t>
+  </si>
+  <si>
+    <t>F2A4D63D5D6FC71892CF5D638A1B4B92F2740D60732F5319A131DF9CA117E5C6</t>
+  </si>
+  <si>
+    <t>FD63CFCF7605F0348435005DED92882D64C10B3C7A26D97AEE39B2D04DF09D1B</t>
+  </si>
+  <si>
+    <t>70D267CBA93577C74A6C6D9A3D17E9FB3929A4E27443873C3821613C15CF949E</t>
+  </si>
+  <si>
+    <t>966BCC126986F4D6ACE6B88296CB12FCBBAB4BF3C39C7482C0D309065674CF94</t>
+  </si>
+  <si>
+    <t>26D789E0CF4E92758BE1E615D989E84D87DF30F932CDBA64A7F1A1E656467437</t>
+  </si>
+  <si>
+    <t>A63C1B5331B78EEE8A48BC910C4002611370D19FD6E8FDD2D89CC3F477ABB28C</t>
+  </si>
+  <si>
+    <t>876D31EB265DD1B36F017DD284FCC6AB4443461B8B840AAD5797533C70245630</t>
+  </si>
+  <si>
+    <t>99031EE03E7D37CBD856A7496FEB6F7B05C0265DAD1F1B10B7C995A72115406C</t>
+  </si>
+  <si>
+    <t>01F0DABD35CEEA103D9E604A6C2859EDEAB10D4EC52AD414B6DD488F723D9FB9</t>
+  </si>
+  <si>
+    <t>6C2C6E77C4EDF27793E30237BD556FCB07A20AFBE125C324ACE5A9572C068F8E</t>
+  </si>
+  <si>
+    <t>E1504D652F794CC5A828E9FE9B162A11998A11E74BC35B5D14098BDD28991E7E</t>
+  </si>
+  <si>
+    <t>F4932F83B82C23FA5A58577FB924E2AC35D71CF8BCE9D3B0A6181056436F78F7</t>
+  </si>
+  <si>
+    <t>39C495BEE03D92EA192B89797D4AFCC98DA6B394E6279426D117EC37AF401A0D</t>
+  </si>
+  <si>
+    <t>53FA5E54F75E5BACB814176DF3F88A78623F79A2F6120168178AA6EE102FD627</t>
+  </si>
+  <si>
+    <t>6540900AE0F7BCC241B19936F3E1CC7E66EA844B8996A0AEA83843B1D364330F</t>
+  </si>
+  <si>
+    <t>31B2A0388E809747941861AE5535827093B535F12B02D93FC56331591475D296</t>
+  </si>
+  <si>
+    <t>FFD7C3067D98579D009DF17F537A658C997AF9A40FAA005164CDE461AEE791DA</t>
   </si>
 </sst>
 </file>
@@ -569,7 +707,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,55 +724,55 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -648,7 +786,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -658,18 +798,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -684,7 +824,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -694,18 +836,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -720,7 +862,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -730,18 +874,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -756,7 +900,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -766,18 +912,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -790,9 +936,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -810,23 +958,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -838,9 +998,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -858,23 +1020,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -886,9 +1060,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -906,23 +1082,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -934,9 +1122,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -954,23 +1144,39 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -982,9 +1188,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1002,23 +1210,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1030,9 +1250,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1050,23 +1272,35 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1094,15 +1328,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1116,9 +1350,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1136,23 +1372,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1164,9 +1428,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1184,23 +1450,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1365,43 +1659,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1432,10 +1726,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1443,16 +1737,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1483,10 +1777,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1494,16 +1788,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1534,10 +1828,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1545,16 +1839,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1586,10 +1880,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1597,31 +1891,72 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1631,54 +1966,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>